<commit_message>
Forecasts and graphs of predictions
</commit_message>
<xml_diff>
--- a/processed_data_ rivero.xlsx
+++ b/processed_data_ rivero.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f44a72708ad2f0af/CC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f44a72708ad2f0af/CC/FINAL_PROJECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_63CAAF6E642AB01DE0D9966ED90A959E9B28D259" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{713D72D4-8E1D-422C-8A02-7573FED46ADE}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_63CAAF6E642AB01DE0D9966ED90A959E9B28D259" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8540018-DDBC-4D80-8D2E-5EFB30DDF53F}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2205" yWindow="2205" windowWidth="16200" windowHeight="9307" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="16200" windowHeight="9307" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Macroeconomic Data" sheetId="1" r:id="rId1"/>
@@ -1948,6 +1948,7 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="59.73046875" customWidth="1"/>
+    <col min="2" max="2" width="18.59765625" customWidth="1"/>
     <col min="5" max="5" width="30.46484375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>